<commit_message>
Màj fichier justifications step 4
</commit_message>
<xml_diff>
--- a/modelisator/Gestion de projet/2015_06_10 [Modelisator] Step 4/2015_06_10 [Modelisator] Todo list.xlsx
+++ b/modelisator/Gestion de projet/2015_06_10 [Modelisator] Step 4/2015_06_10 [Modelisator] Todo list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="4275" yWindow="-180" windowWidth="12390" windowHeight="10050" activeTab="6"/>
@@ -17,7 +17,7 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId8"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1046,9 +1046,24 @@
             <c:strRef>
               <c:f>Feuil1!$B$43:$H$43</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Assistance et maintenance légende Les 4 * 100% 42,5</c:v>
+                  <c:v>Assistance et maintenance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>légende</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Les 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>*</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1087,10 +1102,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -1159,7 +1174,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0,96875</c:v>
+                  <c:v>1,03125</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
@@ -1195,11 +1210,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="74389504"/>
-        <c:axId val="96850432"/>
+        <c:axId val="302136312"/>
+        <c:axId val="302130432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74389504"/>
+        <c:axId val="302136312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1209,7 +1224,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96850432"/>
+        <c:crossAx val="302130432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1217,7 +1232,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96850432"/>
+        <c:axId val="302130432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,7 +1243,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74389504"/>
+        <c:crossAx val="302136312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1275,9 +1290,24 @@
             <c:strRef>
               <c:f>Feuil1!$B$43:$H$43</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Assistance et maintenance légende Les 4 * 100% 42,5</c:v>
+                  <c:v>Assistance et maintenance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>légende</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Les 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>*</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1316,10 +1346,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -1388,7 +1418,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0,96875</c:v>
+                  <c:v>1,03125</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
@@ -1424,11 +1454,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="88016384"/>
-        <c:axId val="96852160"/>
+        <c:axId val="302131608"/>
+        <c:axId val="302132000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88016384"/>
+        <c:axId val="302131608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1438,7 +1468,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96852160"/>
+        <c:crossAx val="302132000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1446,7 +1476,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96852160"/>
+        <c:axId val="302132000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1457,7 +1487,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88016384"/>
+        <c:crossAx val="302131608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1504,9 +1534,24 @@
             <c:strRef>
               <c:f>Feuil1!$B$43:$H$43</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Assistance et maintenance légende Les 4 * 100% 42,5</c:v>
+                  <c:v>Assistance et maintenance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>légende</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Les 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>*</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1545,10 +1590,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -1617,7 +1662,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0,96875</c:v>
+                  <c:v>1,03125</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
@@ -1653,11 +1698,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="88016896"/>
-        <c:axId val="89325568"/>
+        <c:axId val="302132784"/>
+        <c:axId val="302133176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88016896"/>
+        <c:axId val="302132784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1667,7 +1712,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89325568"/>
+        <c:crossAx val="302133176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1675,7 +1720,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89325568"/>
+        <c:axId val="302133176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1686,7 +1731,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88016896"/>
+        <c:crossAx val="302132784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1733,9 +1778,24 @@
             <c:strRef>
               <c:f>Feuil1!$B$43:$H$43</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Assistance et maintenance légende Les 4 * 100% 42,5</c:v>
+                  <c:v>Assistance et maintenance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>légende</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Les 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>*</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1774,10 +1834,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -1846,7 +1906,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0,96875</c:v>
+                  <c:v>1,03125</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
@@ -1882,11 +1942,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="89464832"/>
-        <c:axId val="89327296"/>
+        <c:axId val="302134352"/>
+        <c:axId val="398404064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89464832"/>
+        <c:axId val="302134352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1896,7 +1956,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89327296"/>
+        <c:crossAx val="398404064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1904,7 +1964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89327296"/>
+        <c:axId val="398404064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1915,7 +1975,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89464832"/>
+        <c:crossAx val="302134352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1962,9 +2022,24 @@
             <c:strRef>
               <c:f>Feuil1!$B$43:$H$43</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Assistance et maintenance légende Les 4 * 100% 42,5</c:v>
+                  <c:v>Assistance et maintenance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>légende</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Les 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>*</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2003,10 +2078,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -2075,7 +2150,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0,96875</c:v>
+                  <c:v>1,03125</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
@@ -2111,11 +2186,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="89466368"/>
-        <c:axId val="89329024"/>
+        <c:axId val="398406808"/>
+        <c:axId val="398399360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89466368"/>
+        <c:axId val="398406808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2125,7 +2200,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89329024"/>
+        <c:crossAx val="398399360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2133,7 +2208,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89329024"/>
+        <c:axId val="398399360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2144,7 +2219,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89466368"/>
+        <c:crossAx val="398406808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2191,9 +2266,24 @@
             <c:strRef>
               <c:f>Feuil1!$B$43:$H$43</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>Assistance et maintenance légende Les 4 * 100% 42,5</c:v>
+                  <c:v>Assistance et maintenance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>légende</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Les 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>*</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42,5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2232,10 +2322,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -2304,7 +2394,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0,96875</c:v>
+                  <c:v>1,03125</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0</c:v>
@@ -2340,11 +2430,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="89466880"/>
-        <c:axId val="89330752"/>
+        <c:axId val="398401712"/>
+        <c:axId val="398405632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89466880"/>
+        <c:axId val="398401712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2354,7 +2444,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89330752"/>
+        <c:crossAx val="398405632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2362,7 +2452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89330752"/>
+        <c:axId val="398405632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2373,7 +2463,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89466880"/>
+        <c:crossAx val="398401712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2660,7 +2750,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2695,7 +2785,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2906,8 +2996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3227,7 +3317,7 @@
         <v>0.5</v>
       </c>
       <c r="I12" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -3256,7 +3346,7 @@
         <v>0.5</v>
       </c>
       <c r="I13" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -3826,7 +3916,7 @@
       </c>
       <c r="I36" s="35">
         <f>(SUM(I4:I35)/(COUNT(I4:I35)*3))*3</f>
-        <v>0.96875</v>
+        <v>1.03125</v>
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>

</xml_diff>